<commit_message>
Episode IV: Using the Force
</commit_message>
<xml_diff>
--- a/GeniusSquare_Solve_Prototype.xlsx
+++ b/GeniusSquare_Solve_Prototype.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NoSave\level314\episode\004_PowerOf2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NoSave\level314\src\GenuisSquare\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,8 @@
   <sheets>
     <sheet name="board_calc" sheetId="2" r:id="rId1"/>
     <sheet name="binary" sheetId="1" r:id="rId2"/>
+    <sheet name="stats" sheetId="4" r:id="rId3"/>
+    <sheet name="choose" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Power of 2</t>
   </si>
@@ -66,7 +68,79 @@
     <t>Binary Calculator</t>
   </si>
   <si>
-    <t>O</t>
+    <t>x</t>
+  </si>
+  <si>
+    <t>choose</t>
+  </si>
+  <si>
+    <t>combinations</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>board size</t>
+  </si>
+  <si>
+    <t>sum of games</t>
+  </si>
+  <si>
+    <t>orientations</t>
+  </si>
+  <si>
+    <t>positions per</t>
+  </si>
+  <si>
+    <t>total positions</t>
+  </si>
+  <si>
+    <t>Real Percent</t>
+  </si>
+  <si>
+    <t>reduction</t>
+  </si>
+  <si>
+    <t>Naïve All Possible</t>
+  </si>
+  <si>
+    <t>Estimate Real Possible</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>cyan</t>
+  </si>
+  <si>
+    <t>grey</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t># of pegs</t>
+  </si>
+  <si>
+    <t># of board positions</t>
+  </si>
+  <si>
+    <t># of possible boards</t>
   </si>
 </sst>
 </file>
@@ -77,7 +151,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +176,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,19 +250,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -190,20 +265,28 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -225,6 +308,498 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>choose!$B$3:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>36.000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>630.00000000000034</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58905.000000000015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>376992.00000000012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1947792.0000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8347680.0000000037</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30260340.000000015</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94143280.00000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>254186856.00000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>600805296.00000024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1251677700.0000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2310789600.0000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3796297200.000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5567902560.0000019</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7307872110.0000029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8597496600.0000019</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9075135300.0000019</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8597496600.0000038</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7307872110.0000029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5567902560.0000019</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3796297200.000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2310789600.0000005</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1251677700.0000005</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>600805296.00000036</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>254186856.00000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>94143280.00000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>30260340.000000019</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8347680.0000000028</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1947792.0000000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>376992.00000000006</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>58905.000000000007</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7140</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>630.00000000000034</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36.000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F8AC-4165-A003-562EE6E3791B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="100326784"/>
+        <c:axId val="100951168"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="100326784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100951168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="100951168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100326784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>choose!$C$3:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>1.5563025007672875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7993405494535821</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8536982117761744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7701521603260995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.576332134309987</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.2895425777606153</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9215657924660219</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4808738033730338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.973789325275928</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.4051530894349149</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.7787337522475077</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.0974925148719219</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.3637604042766913</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.5793602046160462</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.7456916263825697</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.8637909384605642</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.9343720127462714</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.9578531085957955</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.9343720127462714</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.8637909384605642</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.7456916263825697</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.5793602046160462</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.3637604042766913</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.0974925148719219</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.7787337522475095</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.4051530894349149</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.973789325275928</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.4808738033730338</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.9215657924660219</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.2895425777606153</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.576332134309987</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.7701521603260995</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.8536982117761744</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.7993405494535821</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.5563025007672875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EF71-44DA-B710-D36991734EA5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="100971264"/>
+        <c:axId val="100972800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="100971264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100972800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="100972800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100971264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -490,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,534 +1077,544 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="I1" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="I1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="Q1" s="10" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="Q1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>5</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>6</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1">
         <v>1</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>2</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>3</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>4</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>5</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>6</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="1">
         <v>2</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
         <v>3</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="1">
         <v>4</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="1">
         <v>5</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="I3" s="2" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="I3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <f>IF(B3&lt;&gt;"", binary!B4, 0)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="2">
         <f>IF(C3&lt;&gt;"", binary!C4, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2">
         <f>IF(D3&lt;&gt;"", binary!D4, 0)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="2">
         <f>IF(E3&lt;&gt;"", binary!E4, 0)</f>
         <v>0</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <f>IF(F3&lt;&gt;"", binary!F4, 0)</f>
-        <v>16</v>
-      </c>
-      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
         <f>IF(G3&lt;&gt;"", binary!G4, 0)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="3" t="str">
+      <c r="R3" s="2" t="str">
         <f>IF(B3="", "0", "1")</f>
         <v>0</v>
       </c>
-      <c r="S3" s="3" t="str">
+      <c r="S3" s="2" t="str">
         <f t="shared" ref="S3:W3" si="0">IF(C3="", "0", "1")</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="3" t="str">
+        <v>1</v>
+      </c>
+      <c r="T3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U3" s="3" t="str">
+      <c r="U3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V3" s="3" t="str">
+      <c r="V3" s="2" t="str">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="I4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <f>IF(B4&lt;&gt;"", binary!B5, 0)</f>
+        <v>64</v>
+      </c>
+      <c r="K4" s="2">
+        <f>IF(C4&lt;&gt;"", binary!C5, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <f>IF(D4&lt;&gt;"", binary!D5, 0)</f>
+        <v>256</v>
+      </c>
+      <c r="M4" s="2">
+        <f>IF(E4&lt;&gt;"", binary!E5, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <f>IF(F4&lt;&gt;"", binary!F5, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <f>IF(G4&lt;&gt;"", binary!G5, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="2" t="str">
+        <f t="shared" ref="R4:R8" si="1">IF(B4="", "0", "1")</f>
         <v>1</v>
       </c>
-      <c r="W3" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
+      <c r="S4" s="2" t="str">
+        <f t="shared" ref="S4:S8" si="2">IF(C4="", "0", "1")</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="str">
+        <f t="shared" ref="T4:T8" si="3">IF(D4="", "0", "1")</f>
+        <v>1</v>
+      </c>
+      <c r="U4" s="2" t="str">
+        <f t="shared" ref="U4:U8" si="4">IF(E4="", "0", "1")</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="str">
+        <f t="shared" ref="V4:V8" si="5">IF(F4="", "0", "1")</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="2" t="str">
+        <f t="shared" ref="W4:W8" si="6">IF(G4="", "0", "1")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="I4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="3">
-        <f>IF(B4&lt;&gt;"", binary!B5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
-        <f>IF(C4&lt;&gt;"", binary!C5, 0)</f>
-        <v>128</v>
-      </c>
-      <c r="L4" s="3">
-        <f>IF(D4&lt;&gt;"", binary!D5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <f>IF(E4&lt;&gt;"", binary!E5, 0)</f>
-        <v>512</v>
-      </c>
-      <c r="N4" s="3">
-        <f>IF(F4&lt;&gt;"", binary!F5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <f>IF(G4&lt;&gt;"", binary!G5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R4" s="3" t="str">
-        <f t="shared" ref="R4:R8" si="1">IF(B4="", "0", "1")</f>
-        <v>0</v>
-      </c>
-      <c r="S4" s="3" t="str">
-        <f t="shared" ref="S4:S8" si="2">IF(C4="", "0", "1")</f>
-        <v>1</v>
-      </c>
-      <c r="T4" s="3" t="str">
-        <f t="shared" ref="T4:T8" si="3">IF(D4="", "0", "1")</f>
-        <v>0</v>
-      </c>
-      <c r="U4" s="3" t="str">
-        <f t="shared" ref="U4:U8" si="4">IF(E4="", "0", "1")</f>
-        <v>1</v>
-      </c>
-      <c r="V4" s="3" t="str">
-        <f t="shared" ref="V4:V8" si="5">IF(F4="", "0", "1")</f>
-        <v>0</v>
-      </c>
-      <c r="W4" s="3" t="str">
-        <f t="shared" ref="W4:W8" si="6">IF(G4="", "0", "1")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <f>IF(B5&lt;&gt;"", binary!B6, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
+        <v>4096</v>
+      </c>
+      <c r="K5" s="2">
         <f>IF(C5&lt;&gt;"", binary!C6, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
+        <v>8192</v>
+      </c>
+      <c r="L5" s="2">
         <f>IF(D5&lt;&gt;"", binary!D6, 0)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <f>IF(E5&lt;&gt;"", binary!E6, 0)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <f>IF(F5&lt;&gt;"", binary!F6, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
+        <v>65536</v>
+      </c>
+      <c r="O5" s="2">
         <f>IF(G5&lt;&gt;"", binary!G6, 0)</f>
         <v>131072</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S5" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T5" s="3" t="str">
+      <c r="R5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S5" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T5" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U5" s="3" t="str">
+      <c r="U5" s="2" t="str">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V5" s="3" t="str">
+      <c r="V5" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W5" s="3" t="str">
+        <v>1</v>
+      </c>
+      <c r="W5" s="2" t="str">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="I6" s="2" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <f>IF(B6&lt;&gt;"", binary!B7, 0)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <f>IF(C6&lt;&gt;"", binary!C7, 0)</f>
-        <v>524288</v>
-      </c>
-      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
         <f>IF(D6&lt;&gt;"", binary!D7, 0)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="2">
         <f>IF(E6&lt;&gt;"", binary!E7, 0)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <f>IF(F6&lt;&gt;"", binary!F7, 0)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="2">
         <f>IF(G6&lt;&gt;"", binary!G7, 0)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S6" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="T6" s="3" t="str">
+      <c r="R6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U6" s="3" t="str">
+      <c r="U6" s="2" t="str">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V6" s="3" t="str">
+      <c r="V6" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W6" s="3" t="str">
+      <c r="W6" s="2" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="I7" s="2" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="I7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <f>IF(B7&lt;&gt;"", binary!B8, 0)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <f>IF(C7&lt;&gt;"", binary!C8, 0)</f>
         <v>0</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <f>IF(D7&lt;&gt;"", binary!D8, 0)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="2">
         <f>IF(E7&lt;&gt;"", binary!E8, 0)</f>
-        <v>134217728</v>
-      </c>
-      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
         <f>IF(F7&lt;&gt;"", binary!F8, 0)</f>
         <v>0</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="2">
         <f>IF(G7&lt;&gt;"", binary!G8, 0)</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R7" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S7" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T7" s="3" t="str">
+      <c r="R7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U7" s="3" t="str">
+      <c r="U7" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V7" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W7" s="3" t="str">
+      <c r="W7" s="2" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="I8" s="2" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="I8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <f>IF(B8&lt;&gt;"", binary!B9, 0)</f>
-        <v>1073741824</v>
-      </c>
-      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
         <f>IF(C8&lt;&gt;"", binary!C9, 0)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <f>IF(D8&lt;&gt;"", binary!D9, 0)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="2">
         <f>IF(E8&lt;&gt;"", binary!E9, 0)</f>
         <v>0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <f>IF(F8&lt;&gt;"", binary!F9, 0)</f>
         <v>0</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="2">
         <f>IF(G8&lt;&gt;"", binary!G9, 0)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R8" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="S8" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T8" s="3" t="str">
+      <c r="R8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="2" t="str">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U8" s="3" t="str">
+      <c r="U8" s="2" t="str">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V8" s="3" t="str">
+      <c r="V8" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W8" s="3" t="str">
+      <c r="W8" s="2" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="13">
         <f>SUM(J3:O8)</f>
-        <v>1208615568</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+        <v>209218</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="12" t="str">
+      <c r="B13" s="9" t="str">
         <f>W8&amp;V8&amp;U8&amp;T8&amp;S8&amp;R8&amp;W7&amp;V7&amp;U7&amp;T7&amp;S7&amp;R7&amp;W6&amp;V6&amp;U6&amp;T6&amp;S6&amp;R6&amp;W5&amp;V5&amp;U5&amp;T5&amp;S5&amp;R5&amp;W4&amp;V4&amp;U4&amp;T4&amp;S4&amp;R4&amp;W3&amp;V3&amp;U3&amp;T3&amp;S3&amp;R3</f>
-        <v>000001001000000010100000001010010000</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+        <v>000000000000000000110011000101000010</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="B14:G14"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B12:G12"/>
-    <mergeCell ref="Q1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1049,254 +1634,254 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>5</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <f>POWER(2,B15)</f>
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <f t="shared" ref="C4:G4" si="0">POWER(2,C15)</f>
         <v>2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <f t="shared" ref="B5:G5" si="1">POWER(2,B16)</f>
         <v>64</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="1"/>
         <v>512</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
         <v>1024</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <f t="shared" ref="B6:G6" si="2">POWER(2,B17)</f>
         <v>4096</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f t="shared" si="2"/>
         <v>8192</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f t="shared" si="2"/>
         <v>16384</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="2"/>
         <v>32768</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f t="shared" si="2"/>
         <v>65536</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f t="shared" si="2"/>
         <v>131072</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <f t="shared" ref="B7:G7" si="3">POWER(2,B18)</f>
         <v>262144</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <f t="shared" si="3"/>
         <v>524288</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <f t="shared" si="3"/>
         <v>1048576</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="3"/>
         <v>2097152</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f t="shared" si="3"/>
         <v>4194304</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f t="shared" si="3"/>
         <v>8388608</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <f t="shared" ref="B8:G8" si="4">POWER(2,B19)</f>
         <v>16777216</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f t="shared" si="4"/>
         <v>33554432</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f t="shared" si="4"/>
         <v>67108864</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="4"/>
         <v>134217728</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f t="shared" si="4"/>
         <v>268435456</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f t="shared" si="4"/>
         <v>536870912</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <f t="shared" ref="B9:G9" si="5">POWER(2,B20)</f>
         <v>1073741824</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <f t="shared" si="5"/>
         <v>2147483648</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <f t="shared" si="5"/>
         <v>4294967296</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="5"/>
         <v>8589934592</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f t="shared" si="5"/>
         <v>17179869184</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f t="shared" si="5"/>
         <v>34359738368</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>3</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>4</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>5</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B15">
@@ -1319,7 +1904,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B16">
@@ -1342,7 +1927,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B17">
@@ -1365,7 +1950,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B18">
@@ -1388,7 +1973,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B19">
@@ -1411,7 +1996,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B20">
@@ -1440,4 +2025,879 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>80</v>
+      </c>
+      <c r="E2">
+        <f>D2*F2</f>
+        <v>80</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.64829999999999999</v>
+      </c>
+      <c r="H2" s="2">
+        <f>D2*D3*D4*D5*D6*D7*D8*D9*D10</f>
+        <v>9555148800000000</v>
+      </c>
+      <c r="I2" s="2">
+        <f>E2*E3*E4*E5*E6*E7*E8*E9*E10</f>
+        <v>11396028999.307137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">B3*C3</f>
+        <v>160</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="1">D3*F3</f>
+        <v>103.72799999999999</v>
+      </c>
+      <c r="F3">
+        <f>G$2*F2</f>
+        <v>0.64829999999999999</v>
+      </c>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>15.130544039999998</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F9" si="2">G$2*F3</f>
+        <v>0.42029288999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>21.798070446959997</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>0.27247588058699995</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>4.4161528346138024</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>0.17664611338455208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>5.4969444147458457</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>0.11451967530720511</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>7.4243105501661075</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>7.4243105501661077E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>2.8879083178036127</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>4.8131805296726879E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>SUM(D2:D10)</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2">
+        <f>FACT(B16)/FACT(B15)/FACT(B16-B15)</f>
+        <v>8347680.0000000037</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <f>FACT(D$2)/FACT(A2)/FACT($D$2-A2)</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>LOG(B2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>36</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7">
+        <f>B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f>FACT(D$2)/FACT(A3)/FACT($D$2-A3)</f>
+        <v>36.000000000000014</v>
+      </c>
+      <c r="C3">
+        <f>LOG(B3)</f>
+        <v>1.5563025007672875</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" s="7">
+        <f t="shared" ref="P3:P9" si="0">B3+P2</f>
+        <v>37.000000000000014</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B38" si="1">FACT(D$2)/FACT(A4)/FACT($D$2-A4)</f>
+        <v>630.00000000000034</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C38" si="2">LOG(B4)</f>
+        <v>2.7993405494535821</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4" s="7">
+        <f t="shared" si="0"/>
+        <v>667.00000000000034</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="1"/>
+        <v>7140</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>3.8536982117761744</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5" s="7">
+        <f t="shared" si="0"/>
+        <v>7807</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="1"/>
+        <v>58905.000000000015</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="2"/>
+        <v>4.7701521603260995</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6" s="7">
+        <f t="shared" si="0"/>
+        <v>66712.000000000015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="1"/>
+        <v>376992.00000000012</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>5.576332134309987</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7" s="7">
+        <f t="shared" si="0"/>
+        <v>443704.00000000012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="1"/>
+        <v>1947792.0000000002</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>6.2895425777606153</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="P8" s="7">
+        <f t="shared" si="0"/>
+        <v>2391496.0000000005</v>
+      </c>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>8347680.0000000037</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>6.9215657924660219</v>
+      </c>
+      <c r="O9">
+        <v>7</v>
+      </c>
+      <c r="P9" s="7">
+        <f t="shared" si="0"/>
+        <v>10739176.000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="1"/>
+        <v>30260340.000000015</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>7.4808738033730338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="1"/>
+        <v>94143280.00000003</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>7.973789325275928</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="1"/>
+        <v>254186856.00000003</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>8.4051530894349149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="1"/>
+        <v>600805296.00000024</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>8.7787337522475077</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="1"/>
+        <v>1251677700.0000005</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>9.0974925148719219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="1"/>
+        <v>2310789600.0000005</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>9.3637604042766913</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="1"/>
+        <v>3796297200.000001</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>9.5793602046160462</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="1"/>
+        <v>5567902560.0000019</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>9.7456916263825697</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="1"/>
+        <v>7307872110.0000029</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>9.8637909384605642</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="1"/>
+        <v>8597496600.0000019</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>9.9343720127462714</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="1"/>
+        <v>9075135300.0000019</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>9.9578531085957955</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="1"/>
+        <v>8597496600.0000038</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>9.9343720127462714</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="1"/>
+        <v>7307872110.0000029</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>9.8637909384605642</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="1"/>
+        <v>5567902560.0000019</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>9.7456916263825697</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="1"/>
+        <v>3796297200.000001</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>9.5793602046160462</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="1"/>
+        <v>2310789600.0000005</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>9.3637604042766913</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="1"/>
+        <v>1251677700.0000005</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>9.0974925148719219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="1"/>
+        <v>600805296.00000036</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>8.7787337522475095</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="1"/>
+        <v>254186856.00000003</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>8.4051530894349149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="1"/>
+        <v>94143280.00000003</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>7.973789325275928</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="1"/>
+        <v>30260340.000000019</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>7.4808738033730338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="1"/>
+        <v>8347680.0000000028</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>6.9215657924660219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" si="1"/>
+        <v>1947792.0000000002</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>6.2895425777606153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2">
+        <f t="shared" si="1"/>
+        <v>376992.00000000006</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>5.576332134309987</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2">
+        <f t="shared" si="1"/>
+        <v>58905.000000000007</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>4.7701521603260995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2">
+        <f t="shared" si="1"/>
+        <v>7140</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>3.8536982117761744</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2">
+        <f t="shared" si="1"/>
+        <v>630.00000000000034</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>2.7993405494535821</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2">
+        <f t="shared" si="1"/>
+        <v>36.000000000000014</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>1.5563025007672875</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>